<commit_message>
generated from ./SC22EVO/HVCB.json at 4381d6c
</commit_message>
<xml_diff>
--- a/SC22EVO/artifacts/HVCB/HVCB.xlsx
+++ b/SC22EVO/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
   <si>
     <t>ID</t>
   </si>
@@ -2801,9 +2801,6 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
-  </si>
-  <si>
-    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29117,7 +29114,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>928</v>
+        <v>863</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29176,7 +29173,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29235,7 +29232,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29294,7 +29291,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29353,7 +29350,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29412,7 +29409,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29439,10 +29436,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="I457" s="6" t="s">
         <v>934</v>
-      </c>
-      <c r="I457" s="6" t="s">
-        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29469,18 +29466,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="U457" s="6" t="s">
         <v>936</v>
-      </c>
-      <c r="U457" s="6" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B458" s="2" t="s">
         <v>938</v>
-      </c>
-      <c r="B458" s="2" t="s">
-        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29498,10 +29495,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="I458" s="2" t="s">
         <v>940</v>
-      </c>
-      <c r="I458" s="2" t="s">
-        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29528,16 +29525,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
+        <v>937</v>
+      </c>
+      <c r="B459" s="5" t="s">
         <v>938</v>
-      </c>
-      <c r="B459" s="5" t="s">
-        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29555,10 +29552,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29585,22 +29582,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>944</v>
       </c>
-      <c r="B460" s="2" t="s">
+      <c r="C460" s="2">
+        <v>0</v>
+      </c>
+      <c r="D460" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="C460" s="2">
-        <v>0</v>
-      </c>
-      <c r="D460" s="2" t="s">
-        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29626,16 +29623,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="B461" s="2" t="s">
         <v>947</v>
       </c>
-      <c r="B461" s="2" t="s">
+      <c r="C461" s="2">
+        <v>0</v>
+      </c>
+      <c r="D461" s="2" t="s">
         <v>948</v>
-      </c>
-      <c r="C461" s="2">
-        <v>0</v>
-      </c>
-      <c r="D461" s="2" t="s">
-        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29661,10 +29658,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>950</v>
-      </c>
-      <c r="B462" s="2" t="s">
-        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29682,7 +29679,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29710,16 +29707,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B463" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B463" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29737,7 +29734,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29761,16 +29758,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B464" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B464" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29788,7 +29785,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29812,16 +29809,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B465" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B465" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29839,7 +29836,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29863,16 +29860,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B466" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B466" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29890,7 +29887,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29914,16 +29911,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B467" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B467" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29941,7 +29938,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29967,16 +29964,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B468" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B468" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29994,7 +29991,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30020,18 +30017,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="U468" s="6" t="s">
         <v>961</v>
-      </c>
-      <c r="U468" s="6" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B469" s="2" t="s">
         <v>963</v>
-      </c>
-      <c r="B469" s="2" t="s">
-        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30049,7 +30046,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30077,16 +30074,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B470" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B470" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30104,7 +30101,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30128,16 +30125,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B471" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B471" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30155,7 +30152,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30179,16 +30176,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B472" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B472" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30206,7 +30203,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30230,16 +30227,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B473" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B473" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30257,7 +30254,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30281,16 +30278,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B474" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B474" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30308,7 +30305,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30334,16 +30331,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B475" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B475" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30361,7 +30358,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30387,18 +30384,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="B476" s="2" t="s">
         <v>974</v>
-      </c>
-      <c r="B476" s="2" t="s">
-        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30416,7 +30413,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30444,16 +30441,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B477" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B477" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30471,7 +30468,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30495,16 +30492,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B478" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B478" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30522,7 +30519,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30546,16 +30543,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B479" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B479" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30573,7 +30570,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30597,16 +30594,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B480" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B480" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30624,7 +30621,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30648,16 +30645,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B481" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B481" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30675,7 +30672,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30701,16 +30698,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B482" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B482" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30728,7 +30725,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30754,18 +30751,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B483" s="2" t="s">
         <v>984</v>
-      </c>
-      <c r="B483" s="2" t="s">
-        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30783,7 +30780,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30811,16 +30808,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B484" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B484" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30838,7 +30835,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30862,16 +30859,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B485" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B485" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30889,7 +30886,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30913,16 +30910,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B486" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B486" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30940,7 +30937,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30964,16 +30961,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B487" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B487" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30991,7 +30988,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31015,16 +31012,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B488" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B488" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31042,7 +31039,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31068,16 +31065,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B489" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B489" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31095,7 +31092,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31121,18 +31118,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B490" s="2" t="s">
         <v>994</v>
-      </c>
-      <c r="B490" s="2" t="s">
-        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31150,7 +31147,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31178,16 +31175,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B491" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B491" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31205,7 +31202,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31229,16 +31226,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B492" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B492" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31256,7 +31253,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31280,16 +31277,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B493" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B493" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31307,7 +31304,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31331,16 +31328,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B494" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B494" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31358,7 +31355,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31382,16 +31379,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B495" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B495" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31409,7 +31406,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31435,16 +31432,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B496" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B496" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31462,7 +31459,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31488,18 +31485,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B497" s="2" t="s">
         <v>1005</v>
-      </c>
-      <c r="B497" s="2" t="s">
-        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31517,7 +31514,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31545,16 +31542,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B498" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B498" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31572,7 +31569,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31596,16 +31593,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B499" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B499" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31623,7 +31620,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31647,16 +31644,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B500" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B500" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31674,7 +31671,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31698,16 +31695,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B501" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B501" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31725,7 +31722,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31749,16 +31746,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B502" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B502" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31776,7 +31773,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31802,16 +31799,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B503" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B503" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31829,7 +31826,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31855,18 +31852,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B504" s="2" t="s">
         <v>1016</v>
-      </c>
-      <c r="B504" s="2" t="s">
-        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31884,7 +31881,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31912,16 +31909,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B505" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B505" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31939,7 +31936,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31963,16 +31960,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B506" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B506" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31990,7 +31987,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32014,16 +32011,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B507" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B507" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32041,7 +32038,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32065,16 +32062,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B508" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B508" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32092,7 +32089,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32116,16 +32113,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B509" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B509" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32143,7 +32140,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32169,16 +32166,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B510" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B510" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32196,7 +32193,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32222,18 +32219,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="U510" s="6" t="s">
         <v>1026</v>
-      </c>
-      <c r="U510" s="6" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B511" s="2" t="s">
         <v>1028</v>
-      </c>
-      <c r="B511" s="2" t="s">
-        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32251,7 +32248,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32279,16 +32276,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B512" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B512" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32306,7 +32303,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32330,16 +32327,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B513" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B513" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32357,7 +32354,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32381,16 +32378,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B514" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B514" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32408,7 +32405,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32432,16 +32429,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B515" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B515" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32459,7 +32456,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32483,16 +32480,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B516" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B516" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32510,7 +32507,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32536,16 +32533,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B517" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B517" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32563,7 +32560,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32589,10 +32586,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC22EVO/HVCB.json at 14aa725
</commit_message>
<xml_diff>
--- a/SC22EVO/artifacts/HVCB/HVCB.xlsx
+++ b/SC22EVO/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
   <si>
     <t>ID</t>
   </si>
@@ -2801,6 +2801,9 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
+  </si>
+  <si>
+    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29114,7 +29117,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>863</v>
+        <v>928</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29173,7 +29176,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29232,7 +29235,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29291,7 +29294,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29350,7 +29353,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29409,7 +29412,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29436,10 +29439,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I457" s="6" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29466,18 +29469,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="U457" s="6" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29495,10 +29498,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="I458" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29525,16 +29528,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29552,10 +29555,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29582,22 +29585,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C460" s="2">
         <v>0</v>
       </c>
       <c r="D460" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29623,16 +29626,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C461" s="2">
         <v>0</v>
       </c>
       <c r="D461" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29658,10 +29661,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29679,7 +29682,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29707,16 +29710,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29734,7 +29737,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29758,16 +29761,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29785,7 +29788,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29809,16 +29812,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29836,7 +29839,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29860,16 +29863,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29887,7 +29890,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29911,16 +29914,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29938,7 +29941,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29964,16 +29967,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29991,7 +29994,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30017,18 +30020,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U468" s="6" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30046,7 +30049,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30074,16 +30077,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30101,7 +30104,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30125,16 +30128,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30152,7 +30155,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30176,16 +30179,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30203,7 +30206,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30227,16 +30230,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30254,7 +30257,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30278,16 +30281,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30305,7 +30308,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30331,16 +30334,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30358,7 +30361,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30384,18 +30387,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30413,7 +30416,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30441,16 +30444,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30468,7 +30471,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30492,16 +30495,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30519,7 +30522,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30543,16 +30546,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30570,7 +30573,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30594,16 +30597,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30621,7 +30624,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30645,16 +30648,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30672,7 +30675,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30698,16 +30701,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30725,7 +30728,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30751,18 +30754,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30780,7 +30783,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30808,16 +30811,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30835,7 +30838,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30859,16 +30862,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30886,7 +30889,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30910,16 +30913,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30937,7 +30940,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30961,16 +30964,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30988,7 +30991,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31012,16 +31015,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31039,7 +31042,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31065,16 +31068,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31092,7 +31095,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31118,18 +31121,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31147,7 +31150,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31175,16 +31178,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31202,7 +31205,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31226,16 +31229,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31253,7 +31256,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31277,16 +31280,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31304,7 +31307,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31328,16 +31331,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31355,7 +31358,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31379,16 +31382,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31406,7 +31409,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31432,16 +31435,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31459,7 +31462,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31485,18 +31488,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31514,7 +31517,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31542,16 +31545,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31569,7 +31572,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31593,16 +31596,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31620,7 +31623,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31644,16 +31647,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31671,7 +31674,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31695,16 +31698,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31722,7 +31725,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31746,16 +31749,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31773,7 +31776,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31799,16 +31802,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31826,7 +31829,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31852,18 +31855,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31881,7 +31884,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31909,16 +31912,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31936,7 +31939,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31960,16 +31963,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B506" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31987,7 +31990,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32011,16 +32014,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32038,7 +32041,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32062,16 +32065,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32089,7 +32092,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32113,16 +32116,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32140,7 +32143,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32166,16 +32169,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32193,7 +32196,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32219,18 +32222,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="U510" s="6" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32248,7 +32251,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32276,16 +32279,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B512" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32303,7 +32306,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32327,16 +32330,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32354,7 +32357,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32378,16 +32381,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32405,7 +32408,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32429,16 +32432,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32456,7 +32459,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32480,16 +32483,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32507,7 +32510,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32533,16 +32536,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32560,7 +32563,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32586,10 +32589,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC22EVO/HVCB.json at fb473e1
</commit_message>
<xml_diff>
--- a/SC22EVO/artifacts/HVCB/HVCB.xlsx
+++ b/SC22EVO/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
   <si>
     <t>ID</t>
   </si>
@@ -2801,9 +2801,6 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
-  </si>
-  <si>
-    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29117,7 +29114,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>928</v>
+        <v>863</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29176,7 +29173,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29235,7 +29232,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29294,7 +29291,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29353,7 +29350,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29412,7 +29409,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29439,10 +29436,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="I457" s="6" t="s">
         <v>934</v>
-      </c>
-      <c r="I457" s="6" t="s">
-        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29469,18 +29466,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="U457" s="6" t="s">
         <v>936</v>
-      </c>
-      <c r="U457" s="6" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B458" s="2" t="s">
         <v>938</v>
-      </c>
-      <c r="B458" s="2" t="s">
-        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29498,10 +29495,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="I458" s="2" t="s">
         <v>940</v>
-      </c>
-      <c r="I458" s="2" t="s">
-        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29528,16 +29525,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
+        <v>937</v>
+      </c>
+      <c r="B459" s="5" t="s">
         <v>938</v>
-      </c>
-      <c r="B459" s="5" t="s">
-        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29555,10 +29552,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29585,22 +29582,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>944</v>
       </c>
-      <c r="B460" s="2" t="s">
+      <c r="C460" s="2">
+        <v>0</v>
+      </c>
+      <c r="D460" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="C460" s="2">
-        <v>0</v>
-      </c>
-      <c r="D460" s="2" t="s">
-        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29626,16 +29623,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="B461" s="2" t="s">
         <v>947</v>
       </c>
-      <c r="B461" s="2" t="s">
+      <c r="C461" s="2">
+        <v>0</v>
+      </c>
+      <c r="D461" s="2" t="s">
         <v>948</v>
-      </c>
-      <c r="C461" s="2">
-        <v>0</v>
-      </c>
-      <c r="D461" s="2" t="s">
-        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29661,10 +29658,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>950</v>
-      </c>
-      <c r="B462" s="2" t="s">
-        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29682,7 +29679,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29710,16 +29707,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B463" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B463" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29737,7 +29734,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29761,16 +29758,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B464" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B464" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29788,7 +29785,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29812,16 +29809,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B465" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B465" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29839,7 +29836,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29863,16 +29860,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B466" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B466" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29890,7 +29887,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29914,16 +29911,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B467" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B467" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29941,7 +29938,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29967,16 +29964,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B468" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B468" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29994,7 +29991,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30020,18 +30017,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="U468" s="6" t="s">
         <v>961</v>
-      </c>
-      <c r="U468" s="6" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B469" s="2" t="s">
         <v>963</v>
-      </c>
-      <c r="B469" s="2" t="s">
-        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30049,7 +30046,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30077,16 +30074,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B470" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B470" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30104,7 +30101,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30128,16 +30125,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B471" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B471" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30155,7 +30152,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30179,16 +30176,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B472" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B472" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30206,7 +30203,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30230,16 +30227,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B473" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B473" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30257,7 +30254,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30281,16 +30278,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B474" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B474" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30308,7 +30305,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30334,16 +30331,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B475" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B475" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30361,7 +30358,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30387,18 +30384,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="B476" s="2" t="s">
         <v>974</v>
-      </c>
-      <c r="B476" s="2" t="s">
-        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30416,7 +30413,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30444,16 +30441,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B477" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B477" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30471,7 +30468,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30495,16 +30492,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B478" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B478" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30522,7 +30519,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30546,16 +30543,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B479" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B479" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30573,7 +30570,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30597,16 +30594,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B480" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B480" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30624,7 +30621,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30648,16 +30645,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B481" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B481" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30675,7 +30672,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30701,16 +30698,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B482" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B482" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30728,7 +30725,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30754,18 +30751,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B483" s="2" t="s">
         <v>984</v>
-      </c>
-      <c r="B483" s="2" t="s">
-        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30783,7 +30780,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30811,16 +30808,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B484" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B484" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30838,7 +30835,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30862,16 +30859,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B485" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B485" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30889,7 +30886,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30913,16 +30910,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B486" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B486" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30940,7 +30937,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30964,16 +30961,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B487" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B487" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30991,7 +30988,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31015,16 +31012,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B488" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B488" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31042,7 +31039,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31068,16 +31065,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B489" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B489" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31095,7 +31092,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31121,18 +31118,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B490" s="2" t="s">
         <v>994</v>
-      </c>
-      <c r="B490" s="2" t="s">
-        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31150,7 +31147,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31178,16 +31175,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B491" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B491" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31205,7 +31202,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31229,16 +31226,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B492" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B492" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31256,7 +31253,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31280,16 +31277,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B493" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B493" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31307,7 +31304,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31331,16 +31328,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B494" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B494" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31358,7 +31355,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31382,16 +31379,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B495" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B495" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31409,7 +31406,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31435,16 +31432,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B496" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B496" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31462,7 +31459,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31488,18 +31485,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B497" s="2" t="s">
         <v>1005</v>
-      </c>
-      <c r="B497" s="2" t="s">
-        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31517,7 +31514,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31545,16 +31542,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B498" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B498" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31572,7 +31569,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31596,16 +31593,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B499" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B499" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31623,7 +31620,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31647,16 +31644,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B500" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B500" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31674,7 +31671,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31698,16 +31695,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B501" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B501" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31725,7 +31722,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31749,16 +31746,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B502" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B502" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31776,7 +31773,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31802,16 +31799,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B503" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B503" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31829,7 +31826,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31855,18 +31852,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B504" s="2" t="s">
         <v>1016</v>
-      </c>
-      <c r="B504" s="2" t="s">
-        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31884,7 +31881,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31912,16 +31909,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B505" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B505" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31939,7 +31936,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31963,16 +31960,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B506" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B506" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31990,7 +31987,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32014,16 +32011,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B507" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B507" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32041,7 +32038,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32065,16 +32062,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B508" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B508" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32092,7 +32089,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32116,16 +32113,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B509" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B509" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32143,7 +32140,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32169,16 +32166,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B510" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B510" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32196,7 +32193,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32222,18 +32219,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="U510" s="6" t="s">
         <v>1026</v>
-      </c>
-      <c r="U510" s="6" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B511" s="2" t="s">
         <v>1028</v>
-      </c>
-      <c r="B511" s="2" t="s">
-        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32251,7 +32248,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32279,16 +32276,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B512" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B512" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32306,7 +32303,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32330,16 +32327,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B513" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B513" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32357,7 +32354,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32381,16 +32378,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B514" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B514" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32408,7 +32405,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32432,16 +32429,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B515" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B515" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32459,7 +32456,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32483,16 +32480,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B516" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B516" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32510,7 +32507,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32536,16 +32533,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B517" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B517" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32563,7 +32560,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32589,10 +32586,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC22EVO/HVCB.json at e2baa35
</commit_message>
<xml_diff>
--- a/SC22EVO/artifacts/HVCB/HVCB.xlsx
+++ b/SC22EVO/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
   <si>
     <t>ID</t>
   </si>
@@ -2801,6 +2801,9 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
+  </si>
+  <si>
+    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29114,7 +29117,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>863</v>
+        <v>928</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29173,7 +29176,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29232,7 +29235,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29291,7 +29294,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29350,7 +29353,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29409,7 +29412,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29436,10 +29439,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I457" s="6" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29466,18 +29469,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="U457" s="6" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29495,10 +29498,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="I458" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29525,16 +29528,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29552,10 +29555,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29582,22 +29585,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C460" s="2">
         <v>0</v>
       </c>
       <c r="D460" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29623,16 +29626,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C461" s="2">
         <v>0</v>
       </c>
       <c r="D461" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29658,10 +29661,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29679,7 +29682,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29707,16 +29710,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29734,7 +29737,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29758,16 +29761,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29785,7 +29788,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29809,16 +29812,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29836,7 +29839,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29860,16 +29863,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29887,7 +29890,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29911,16 +29914,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29938,7 +29941,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29964,16 +29967,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29991,7 +29994,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30017,18 +30020,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U468" s="6" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30046,7 +30049,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30074,16 +30077,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30101,7 +30104,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30125,16 +30128,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30152,7 +30155,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30176,16 +30179,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30203,7 +30206,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30227,16 +30230,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30254,7 +30257,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30278,16 +30281,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30305,7 +30308,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30331,16 +30334,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30358,7 +30361,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30384,18 +30387,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30413,7 +30416,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30441,16 +30444,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30468,7 +30471,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30492,16 +30495,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30519,7 +30522,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30543,16 +30546,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30570,7 +30573,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30594,16 +30597,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30621,7 +30624,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30645,16 +30648,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30672,7 +30675,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30698,16 +30701,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30725,7 +30728,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30751,18 +30754,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30780,7 +30783,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30808,16 +30811,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30835,7 +30838,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30859,16 +30862,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30886,7 +30889,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30910,16 +30913,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30937,7 +30940,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30961,16 +30964,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30988,7 +30991,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31012,16 +31015,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31039,7 +31042,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31065,16 +31068,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31092,7 +31095,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31118,18 +31121,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31147,7 +31150,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31175,16 +31178,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31202,7 +31205,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31226,16 +31229,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31253,7 +31256,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31277,16 +31280,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31304,7 +31307,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31328,16 +31331,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31355,7 +31358,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31379,16 +31382,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31406,7 +31409,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31432,16 +31435,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31459,7 +31462,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31485,18 +31488,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31514,7 +31517,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31542,16 +31545,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31569,7 +31572,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31593,16 +31596,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31620,7 +31623,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31644,16 +31647,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31671,7 +31674,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31695,16 +31698,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31722,7 +31725,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31746,16 +31749,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31773,7 +31776,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31799,16 +31802,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31826,7 +31829,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31852,18 +31855,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31881,7 +31884,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31909,16 +31912,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31936,7 +31939,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31960,16 +31963,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B506" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31987,7 +31990,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32011,16 +32014,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32038,7 +32041,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32062,16 +32065,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32089,7 +32092,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32113,16 +32116,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32140,7 +32143,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32166,16 +32169,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32193,7 +32196,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32219,18 +32222,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="U510" s="6" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32248,7 +32251,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32276,16 +32279,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B512" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32303,7 +32306,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32327,16 +32330,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32354,7 +32357,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32378,16 +32381,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32405,7 +32408,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32429,16 +32432,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32456,7 +32459,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32480,16 +32483,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32507,7 +32510,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32533,16 +32536,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32560,7 +32563,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32586,10 +32589,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC22EVO/HVCB.json at 2c48e30
</commit_message>
<xml_diff>
--- a/SC22EVO/artifacts/HVCB/HVCB.xlsx
+++ b/SC22EVO/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
   <si>
     <t>ID</t>
   </si>
@@ -2801,9 +2801,6 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
-  </si>
-  <si>
-    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29117,7 +29114,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>928</v>
+        <v>863</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29176,7 +29173,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29235,7 +29232,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29294,7 +29291,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29353,7 +29350,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29412,7 +29409,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29439,10 +29436,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="I457" s="6" t="s">
         <v>934</v>
-      </c>
-      <c r="I457" s="6" t="s">
-        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29469,18 +29466,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="U457" s="6" t="s">
         <v>936</v>
-      </c>
-      <c r="U457" s="6" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B458" s="2" t="s">
         <v>938</v>
-      </c>
-      <c r="B458" s="2" t="s">
-        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29498,10 +29495,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="I458" s="2" t="s">
         <v>940</v>
-      </c>
-      <c r="I458" s="2" t="s">
-        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29528,16 +29525,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
+        <v>937</v>
+      </c>
+      <c r="B459" s="5" t="s">
         <v>938</v>
-      </c>
-      <c r="B459" s="5" t="s">
-        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29555,10 +29552,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29585,22 +29582,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>944</v>
       </c>
-      <c r="B460" s="2" t="s">
+      <c r="C460" s="2">
+        <v>0</v>
+      </c>
+      <c r="D460" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="C460" s="2">
-        <v>0</v>
-      </c>
-      <c r="D460" s="2" t="s">
-        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29626,16 +29623,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="B461" s="2" t="s">
         <v>947</v>
       </c>
-      <c r="B461" s="2" t="s">
+      <c r="C461" s="2">
+        <v>0</v>
+      </c>
+      <c r="D461" s="2" t="s">
         <v>948</v>
-      </c>
-      <c r="C461" s="2">
-        <v>0</v>
-      </c>
-      <c r="D461" s="2" t="s">
-        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29661,10 +29658,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>950</v>
-      </c>
-      <c r="B462" s="2" t="s">
-        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29682,7 +29679,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29710,16 +29707,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B463" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B463" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29737,7 +29734,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29761,16 +29758,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B464" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B464" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29788,7 +29785,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29812,16 +29809,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B465" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B465" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29839,7 +29836,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29863,16 +29860,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B466" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B466" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29890,7 +29887,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29914,16 +29911,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B467" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B467" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29941,7 +29938,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29967,16 +29964,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B468" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B468" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29994,7 +29991,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30020,18 +30017,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="U468" s="6" t="s">
         <v>961</v>
-      </c>
-      <c r="U468" s="6" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B469" s="2" t="s">
         <v>963</v>
-      </c>
-      <c r="B469" s="2" t="s">
-        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30049,7 +30046,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30077,16 +30074,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B470" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B470" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30104,7 +30101,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30128,16 +30125,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B471" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B471" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30155,7 +30152,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30179,16 +30176,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B472" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B472" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30206,7 +30203,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30230,16 +30227,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B473" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B473" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30257,7 +30254,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30281,16 +30278,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B474" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B474" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30308,7 +30305,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30334,16 +30331,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B475" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B475" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30361,7 +30358,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30387,18 +30384,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="B476" s="2" t="s">
         <v>974</v>
-      </c>
-      <c r="B476" s="2" t="s">
-        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30416,7 +30413,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30444,16 +30441,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B477" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B477" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30471,7 +30468,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30495,16 +30492,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B478" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B478" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30522,7 +30519,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30546,16 +30543,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B479" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B479" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30573,7 +30570,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30597,16 +30594,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B480" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B480" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30624,7 +30621,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30648,16 +30645,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B481" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B481" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30675,7 +30672,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30701,16 +30698,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B482" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B482" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30728,7 +30725,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30754,18 +30751,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B483" s="2" t="s">
         <v>984</v>
-      </c>
-      <c r="B483" s="2" t="s">
-        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30783,7 +30780,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30811,16 +30808,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B484" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B484" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30838,7 +30835,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30862,16 +30859,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B485" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B485" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30889,7 +30886,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30913,16 +30910,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B486" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B486" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30940,7 +30937,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30964,16 +30961,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B487" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B487" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30991,7 +30988,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31015,16 +31012,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B488" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B488" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31042,7 +31039,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31068,16 +31065,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B489" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B489" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31095,7 +31092,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31121,18 +31118,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B490" s="2" t="s">
         <v>994</v>
-      </c>
-      <c r="B490" s="2" t="s">
-        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31150,7 +31147,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31178,16 +31175,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B491" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B491" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31205,7 +31202,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31229,16 +31226,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B492" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B492" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31256,7 +31253,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31280,16 +31277,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B493" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B493" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31307,7 +31304,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31331,16 +31328,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B494" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B494" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31358,7 +31355,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31382,16 +31379,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B495" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B495" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31409,7 +31406,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31435,16 +31432,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B496" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B496" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31462,7 +31459,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31488,18 +31485,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B497" s="2" t="s">
         <v>1005</v>
-      </c>
-      <c r="B497" s="2" t="s">
-        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31517,7 +31514,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31545,16 +31542,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B498" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B498" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31572,7 +31569,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31596,16 +31593,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B499" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B499" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31623,7 +31620,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31647,16 +31644,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B500" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B500" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31674,7 +31671,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31698,16 +31695,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B501" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B501" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31725,7 +31722,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31749,16 +31746,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B502" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B502" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31776,7 +31773,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31802,16 +31799,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B503" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B503" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31829,7 +31826,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31855,18 +31852,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B504" s="2" t="s">
         <v>1016</v>
-      </c>
-      <c r="B504" s="2" t="s">
-        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31884,7 +31881,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31912,16 +31909,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B505" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B505" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31939,7 +31936,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31963,16 +31960,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B506" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B506" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31990,7 +31987,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32014,16 +32011,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B507" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B507" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32041,7 +32038,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32065,16 +32062,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B508" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B508" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32092,7 +32089,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32116,16 +32113,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B509" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B509" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32143,7 +32140,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32169,16 +32166,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B510" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B510" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32196,7 +32193,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32222,18 +32219,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="U510" s="6" t="s">
         <v>1026</v>
-      </c>
-      <c r="U510" s="6" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B511" s="2" t="s">
         <v>1028</v>
-      </c>
-      <c r="B511" s="2" t="s">
-        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32251,7 +32248,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32279,16 +32276,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B512" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B512" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32306,7 +32303,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32330,16 +32327,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B513" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B513" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32357,7 +32354,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32381,16 +32378,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B514" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B514" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32408,7 +32405,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32432,16 +32429,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B515" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B515" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32459,7 +32456,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32483,16 +32480,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B516" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B516" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32510,7 +32507,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32536,16 +32533,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B517" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B517" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32563,7 +32560,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32589,10 +32586,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>